<commit_message>
organize all the things
</commit_message>
<xml_diff>
--- a/data/kimse2020viral/asymptomatic.xlsx
+++ b/data/kimse2020viral/asymptomatic.xlsx
@@ -27,130 +27,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="14">
   <si>
-    <t>Patient</t>
+    <t>PatientID</t>
   </si>
   <si>
-    <t xml:space="preserve">Age </t>
+    <t>day</t>
   </si>
   <si>
-    <t>Sex</t>
+    <t>value</t>
   </si>
   <si>
-    <t>Underlying disease</t>
+    <t>viral load</t>
   </si>
   <si>
-    <t>Contact with confirmed COVID-19 case</t>
+    <t>4-4</t>
   </si>
   <si>
-    <t>Incubation perioda(days)</t>
+    <t>4-5</t>
   </si>
   <si>
-    <t>Symptom-free period after admission (days)</t>
+    <t>4-6</t>
   </si>
   <si>
-    <t>Maximal O^2
-supply (min/l)</t>
+    <t>4-7</t>
   </si>
   <si>
-    <t>Pneumonia extent (max 24)</t>
+    <t>4-8</t>
   </si>
   <si>
-    <t>Treatment</t>
+    <t>4-9</t>
   </si>
   <si>
-    <t>A</t>
+    <t>4-10</t>
   </si>
   <si>
-    <t>F</t>
+    <t>4-11</t>
   </si>
   <si>
-    <t>None</t>
+    <t>4-12</t>
   </si>
   <si>
-    <t>Family</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>LPV/r</t>
-  </si>
-  <si>
-    <t> B</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>Religious event</t>
-  </si>
-  <si>
-    <t> C</t>
-  </si>
-  <si>
-    <t>HTN</t>
-  </si>
-  <si>
-    <t> D</t>
-  </si>
-  <si>
-    <t>DM</t>
-  </si>
-  <si>
-    <t> E</t>
-  </si>
-  <si>
-    <t>Asthma, osteoporosis</t>
-  </si>
-  <si>
-    <t>Medical care</t>
-  </si>
-  <si>
-    <t> F</t>
-  </si>
-  <si>
-    <t>Foreign visit, family</t>
-  </si>
-  <si>
-    <t> G</t>
-  </si>
-  <si>
-    <t>Liver donor</t>
-  </si>
-  <si>
-    <t>Foreign visit</t>
-  </si>
-  <si>
-    <t>14b</t>
-  </si>
-  <si>
-    <t> H</t>
-  </si>
-  <si>
-    <t> I</t>
-  </si>
-  <si>
-    <t>20b</t>
-  </si>
-  <si>
-    <t> J</t>
-  </si>
-  <si>
-    <t> K</t>
-  </si>
-  <si>
-    <t>Dormitory</t>
-  </si>
-  <si>
-    <t> L</t>
-  </si>
-  <si>
-    <t>Occupational</t>
-  </si>
-  <si>
-    <t> M</t>
+    <t>4-13</t>
   </si>
 </sst>
 </file>
@@ -163,17 +81,10 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13.1"/>
-      <color rgb="FF1B1B1B"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -643,133 +554,133 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -777,11 +688,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1058,59 +969,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>118745</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>100330</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="309880" cy="286385"/>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="文本框 1"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9733915" y="3313430"/>
-          <a:ext cx="309880" cy="286385"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="WPS">
   <a:themeElements>
@@ -1361,480 +1219,596 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="3"/>
   <cols>
-    <col min="4" max="4" width="19.5480769230769" customWidth="1"/>
-    <col min="5" max="5" width="13.9326923076923" customWidth="1"/>
-    <col min="6" max="6" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="16.6538461538462" customWidth="1"/>
-    <col min="8" max="8" width="18.4230769230769" customWidth="1"/>
-    <col min="9" max="9" width="17.7788461538462" customWidth="1"/>
-    <col min="10" max="10" width="15.0673076923077" customWidth="1"/>
+    <col min="1" max="1" width="9.23076923076923" style="1"/>
+    <col min="2" max="2" width="21.9519230769231" customWidth="1"/>
+    <col min="3" max="3" width="27.7211538461538" customWidth="1"/>
+    <col min="4" max="4" width="15.0576923076923" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="96" spans="1:10">
+    <row r="1" ht="15" customHeight="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B2">
+        <v>2.96714129244249</v>
+      </c>
+      <c r="C2">
+        <v>32.8626732635872</v>
+      </c>
+      <c r="D2">
+        <v>4.023755</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>4.99123767798466</v>
+      </c>
+      <c r="C3">
+        <v>39.8686281174856</v>
+      </c>
+      <c r="D3">
+        <v>1.868053</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>6.96933187294633</v>
+      </c>
+      <c r="C4">
+        <v>35.8976973725623</v>
+      </c>
+      <c r="D4">
+        <v>3.089891</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>8.9934282584885</v>
+      </c>
+      <c r="C5">
+        <v>32.8461809620928</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4.028829</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>11.0175246440306</v>
+      </c>
+      <c r="C6">
+        <v>33.9325955861061</v>
+      </c>
+      <c r="D6">
+        <v>3.694544</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>12.9956188389923</v>
+      </c>
+      <c r="C7">
+        <v>39.7892510480794</v>
+      </c>
+      <c r="D7">
+        <v>1.892477</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>14.9967141292442</v>
+      </c>
+      <c r="C8">
+        <v>39.8412458611877</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.876479</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>17.0438116100766</v>
+      </c>
+      <c r="C9">
+        <v>36.8471377673704</v>
+      </c>
+      <c r="D9">
+        <v>2.797753</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>18.998904709748</v>
+      </c>
+      <c r="C10">
+        <v>39.8877642230363</v>
+      </c>
+      <c r="D10">
+        <v>1.862165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>21.0230010952902</v>
+      </c>
+      <c r="C11">
+        <v>39.8247535596933</v>
+      </c>
+      <c r="D11">
+        <v>1.881553</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B12">
+        <v>8.02738225629792</v>
+      </c>
+      <c r="C12">
+        <v>33.8258362604021</v>
+      </c>
+      <c r="D12">
+        <v>3.727394</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>10.0284775465498</v>
+      </c>
+      <c r="C13">
+        <v>39.8548425677632</v>
+      </c>
+      <c r="D13">
+        <v>1.872295</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B14">
+        <v>2.00109529025191</v>
+      </c>
+      <c r="C14">
+        <v>39.9342825848849</v>
+      </c>
+      <c r="D14">
+        <v>1.847852</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>3.03614457831325</v>
+      </c>
+      <c r="C15">
+        <v>40.0463924664173</v>
+      </c>
+      <c r="D15">
+        <v>1.813356</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B16">
+        <v>0.966046002190581</v>
+      </c>
+      <c r="C16">
+        <v>34.7072301746169</v>
+      </c>
+      <c r="D16">
+        <v>3.456193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <v>1.97809419496166</v>
+      </c>
+      <c r="C17">
+        <v>39.8768742682328</v>
+      </c>
+      <c r="D17">
+        <v>1.865516</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <v>3.013143483023</v>
+      </c>
+      <c r="C18">
+        <v>39.8165703566617</v>
+      </c>
+      <c r="D18">
+        <v>1.884071</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>4.02519167579408</v>
+      </c>
+      <c r="C19">
+        <v>39.8138006571741</v>
+      </c>
+      <c r="D19">
+        <v>1.884924</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>5.01423877327491</v>
+      </c>
+      <c r="C20">
+        <v>34.8685651697699</v>
+      </c>
+      <c r="D20">
+        <v>3.406551</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="B21">
+        <v>2.00109529025191</v>
+      </c>
+      <c r="C21">
+        <v>26.8883055733907</v>
+      </c>
+      <c r="D21">
+        <v>5.862042</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22">
+        <v>3.97918948521358</v>
+      </c>
+      <c r="C22">
+        <v>35.848409311226</v>
+      </c>
+      <c r="D22">
+        <v>3.105057</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>7.03833515881708</v>
+      </c>
+      <c r="C23">
+        <v>39.9204970351625</v>
+      </c>
+      <c r="D23">
+        <v>1.852094</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" ht="20" spans="1:10">
-      <c r="A2" s="2" t="s">
+      <c r="B24">
+        <v>2.00109529025191</v>
+      </c>
+      <c r="C24">
+        <v>36.9457768377585</v>
+      </c>
+      <c r="D24">
+        <v>2.767402</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>4.00219058050383</v>
+      </c>
+      <c r="C25">
+        <v>39.9862773979932</v>
+      </c>
+      <c r="D25">
+        <v>1.831853</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2">
-        <v>20</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B26">
+        <v>4.00219058050383</v>
+      </c>
+      <c r="C26">
+        <v>39.9288061336254</v>
+      </c>
+      <c r="D26">
+        <v>1.849537</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="B27">
+        <v>0.989047097480832</v>
+      </c>
+      <c r="C27">
+        <v>24.0175120544875</v>
+      </c>
+      <c r="D27">
+        <v>6.745372</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28">
+        <v>2.99014238773274</v>
+      </c>
+      <c r="C28">
+        <v>34.0695068675957</v>
+      </c>
+      <c r="D28">
+        <v>3.652417</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29">
+        <v>4.99123767798466</v>
+      </c>
+      <c r="C29">
+        <v>38.9490878876005</v>
+      </c>
+      <c r="D29">
+        <v>2.150992</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30">
+        <v>6.99233296823658</v>
+      </c>
+      <c r="C30">
+        <v>40.0930367236972</v>
+      </c>
+      <c r="D30">
+        <v>1.799004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="B31">
+        <v>8.00438116100766</v>
+      </c>
+      <c r="C31">
+        <v>31.8718762196119</v>
+      </c>
+      <c r="D31">
+        <v>4.328619</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32">
+        <v>9.98247535596933</v>
+      </c>
+      <c r="C32">
+        <v>29.7974971988266</v>
+      </c>
+      <c r="D32">
+        <v>4.966896</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33">
+        <v>11.9835706462212</v>
+      </c>
+      <c r="C33">
+        <v>34.792020747567</v>
+      </c>
+      <c r="D33">
+        <v>3.430103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34">
+        <v>14.0306681270536</v>
+      </c>
+      <c r="C34">
+        <v>39.843889665244</v>
+      </c>
+      <c r="D34">
+        <v>1.875665</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35">
+        <v>16.0087623220153</v>
+      </c>
+      <c r="C35">
+        <v>39.8384761617</v>
+      </c>
+      <c r="D35">
+        <v>1.877331</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="2">
-        <v>2</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" ht="39" spans="1:10">
-      <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="2">
-        <v>30</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="2">
-        <v>4</v>
-      </c>
-      <c r="G3" s="2">
-        <v>2</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" ht="39" customHeight="1" spans="1:10">
-      <c r="A4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="2">
-        <v>30</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="2">
-        <v>4</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" ht="20" spans="1:10">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2">
-        <v>58</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="B36">
+        <v>1.97809419496166</v>
+      </c>
+      <c r="C36">
+        <v>27.922851279727</v>
+      </c>
+      <c r="D36">
+        <v>5.543716</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="2">
-        <v>2</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" ht="39" spans="1:10">
-      <c r="A6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="2">
-        <v>79</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="2">
-        <v>10</v>
-      </c>
-      <c r="G6" s="2">
-        <v>7</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" ht="39" spans="1:10">
-      <c r="A7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="2">
-        <v>8</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="2">
-        <v>2</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" ht="20" spans="1:10">
-      <c r="A8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="2">
-        <v>37</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2">
-        <v>0</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" ht="39" spans="1:10">
-      <c r="A9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="2">
-        <v>48</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="2">
-        <v>2</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" ht="39" spans="1:10">
-      <c r="A10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="2">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="2">
-        <v>1</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" ht="20" spans="1:10">
-      <c r="A11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="2">
-        <v>8</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="B37">
+        <v>4.00219058050383</v>
+      </c>
+      <c r="C37">
+        <v>31.9403003864989</v>
+      </c>
+      <c r="D37">
+        <v>4.307565</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="2">
-        <v>2</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" ht="20" spans="1:10">
-      <c r="A12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="2">
-        <v>21</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" ht="39" spans="1:10">
-      <c r="A13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="2">
-        <v>55</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="2">
-        <v>10</v>
-      </c>
-      <c r="G13" s="2">
-        <v>7</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" ht="20" spans="1:10">
-      <c r="A14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="2">
-        <v>25</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="2">
-        <v>1</v>
-      </c>
-      <c r="H14" s="2">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>12</v>
+      <c r="B38">
+        <v>6.026286966046</v>
+      </c>
+      <c r="C38">
+        <v>33.9462552403973</v>
+      </c>
+      <c r="D38">
+        <v>3.690341</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39">
+        <v>8.02738225629792</v>
+      </c>
+      <c r="C39">
+        <v>35.8948017776434</v>
+      </c>
+      <c r="D39">
+        <v>3.090782</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40">
+        <v>8.9934282584885</v>
+      </c>
+      <c r="C40">
+        <v>32.8461809620928</v>
+      </c>
+      <c r="D40">
+        <v>4.028829</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41">
+        <v>11.0175246440306</v>
+      </c>
+      <c r="C41">
+        <v>39.909607080359</v>
+      </c>
+      <c r="D41">
+        <v>1.855444</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F1" r:id="rId2" location="tblfn0005" display="Incubation perioda(days)"/>
-    <hyperlink ref="F8" r:id="rId2" location="tblfn0010" display="14b"/>
-    <hyperlink ref="F10" r:id="rId2" location="tblfn0010" display="20b"/>
-    <hyperlink ref="F12" r:id="rId2" location="tblfn0010" display="14b"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change md file and update yaml file
</commit_message>
<xml_diff>
--- a/data/kimse2020viral/asymptomatic.xlsx
+++ b/data/kimse2020viral/asymptomatic.xlsx
@@ -27,12 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="18">
   <si>
     <t>PatientID</t>
   </si>
   <si>
-    <t>day</t>
+    <t>Day</t>
   </si>
   <si>
     <t>value</t>
@@ -41,10 +41,22 @@
     <t>viral load</t>
   </si>
   <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
     <t>4-4</t>
   </si>
   <si>
+    <t>M</t>
+  </si>
+  <si>
     <t>4-5</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
   <si>
     <t>4-6</t>
@@ -81,10 +93,17 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13.1"/>
+      <color rgb="FF1B1B1B"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -554,137 +573,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -693,6 +712,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1219,13 +1244,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <cols>
     <col min="1" max="1" width="9.23076923076923" style="1"/>
     <col min="2" max="2" width="21.9519230769231" customWidth="1"/>
@@ -1233,7 +1258,7 @@
     <col min="4" max="4" width="15.0576923076923" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" spans="1:4">
+    <row r="1" ht="15" customHeight="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1246,10 +1271,18 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" ht="19.2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>2.96714129244249</v>
@@ -1260,10 +1293,18 @@
       <c r="D2">
         <v>4.023755</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>58</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" ht="19.2" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>4.99123767798466</v>
@@ -1274,10 +1315,18 @@
       <c r="D3">
         <v>1.868053</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" ht="19.2" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>6.96933187294633</v>
@@ -1288,10 +1337,18 @@
       <c r="D4">
         <v>3.089891</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>58</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" ht="19.2" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>8.9934282584885</v>
@@ -1302,10 +1359,18 @@
       <c r="D5" s="2">
         <v>4.028829</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>58</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" ht="19.2" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>11.0175246440306</v>
@@ -1316,10 +1381,18 @@
       <c r="D6">
         <v>3.694544</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>58</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" ht="19.2" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>12.9956188389923</v>
@@ -1330,10 +1403,18 @@
       <c r="D7">
         <v>1.892477</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>58</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" ht="19.2" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>14.9967141292442</v>
@@ -1344,10 +1425,18 @@
       <c r="D8" s="2">
         <v>1.876479</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8">
+        <v>58</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" ht="19.2" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>17.0438116100766</v>
@@ -1358,10 +1447,18 @@
       <c r="D9">
         <v>2.797753</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>58</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" ht="19.2" spans="1:9">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>18.998904709748</v>
@@ -1372,10 +1469,18 @@
       <c r="D10">
         <v>1.862165</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10">
+        <v>58</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" ht="19.2" spans="1:9">
       <c r="A11" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B11">
         <v>21.0230010952902</v>
@@ -1386,10 +1491,18 @@
       <c r="D11">
         <v>1.881553</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <v>58</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" ht="19.2" spans="1:9">
       <c r="A12" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>8.02738225629792</v>
@@ -1400,10 +1513,18 @@
       <c r="D12">
         <v>3.727394</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <v>79</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" ht="19.2" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <v>10.0284775465498</v>
@@ -1414,10 +1535,18 @@
       <c r="D13">
         <v>1.872295</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13">
+        <v>79</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" ht="19.2" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>2.00109529025191</v>
@@ -1428,10 +1557,18 @@
       <c r="D14">
         <v>1.847852</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B15">
         <v>3.03614457831325</v>
@@ -1442,10 +1579,16 @@
       <c r="D15">
         <v>1.813356</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B16">
         <v>0.966046002190581</v>
@@ -1456,10 +1599,16 @@
       <c r="D16">
         <v>3.456193</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>37</v>
+      </c>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B17">
         <v>1.97809419496166</v>
@@ -1470,10 +1619,16 @@
       <c r="D17">
         <v>1.865516</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>37</v>
+      </c>
+      <c r="F17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B18">
         <v>3.013143483023</v>
@@ -1484,10 +1639,16 @@
       <c r="D18">
         <v>1.884071</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <v>37</v>
+      </c>
+      <c r="F18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B19">
         <v>4.02519167579408</v>
@@ -1498,10 +1659,16 @@
       <c r="D19">
         <v>1.884924</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19">
+        <v>37</v>
+      </c>
+      <c r="F19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B20">
         <v>5.01423877327491</v>
@@ -1512,10 +1679,16 @@
       <c r="D20">
         <v>3.406551</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20">
+        <v>37</v>
+      </c>
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B21">
         <v>2.00109529025191</v>
@@ -1526,10 +1699,16 @@
       <c r="D21">
         <v>5.862042</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21">
+        <v>48</v>
+      </c>
+      <c r="F21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B22">
         <v>3.97918948521358</v>
@@ -1540,10 +1719,16 @@
       <c r="D22">
         <v>3.105057</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22">
+        <v>48</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B23">
         <v>7.03833515881708</v>
@@ -1554,10 +1739,16 @@
       <c r="D23">
         <v>1.852094</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23">
+        <v>48</v>
+      </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B24">
         <v>2.00109529025191</v>
@@ -1568,10 +1759,16 @@
       <c r="D24">
         <v>2.767402</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24">
+        <v>24</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B25">
         <v>4.00219058050383</v>
@@ -1582,10 +1779,16 @@
       <c r="D25">
         <v>1.831853</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25">
+        <v>24</v>
+      </c>
+      <c r="F25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B26">
         <v>4.00219058050383</v>
@@ -1596,10 +1799,16 @@
       <c r="D26">
         <v>1.849537</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26">
+        <v>8</v>
+      </c>
+      <c r="F26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B27">
         <v>0.989047097480832</v>
@@ -1610,10 +1819,16 @@
       <c r="D27">
         <v>6.745372</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27">
+        <v>21</v>
+      </c>
+      <c r="F27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B28">
         <v>2.99014238773274</v>
@@ -1624,10 +1839,16 @@
       <c r="D28">
         <v>3.652417</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28">
+        <v>21</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B29">
         <v>4.99123767798466</v>
@@ -1638,10 +1859,16 @@
       <c r="D29">
         <v>2.150992</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29">
+        <v>21</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B30">
         <v>6.99233296823658</v>
@@ -1652,10 +1879,16 @@
       <c r="D30">
         <v>1.799004</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30">
+        <v>21</v>
+      </c>
+      <c r="F30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B31">
         <v>8.00438116100766</v>
@@ -1666,10 +1899,16 @@
       <c r="D31">
         <v>4.328619</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31">
+        <v>55</v>
+      </c>
+      <c r="F31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B32">
         <v>9.98247535596933</v>
@@ -1680,10 +1919,16 @@
       <c r="D32">
         <v>4.966896</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32">
+        <v>55</v>
+      </c>
+      <c r="F32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B33">
         <v>11.9835706462212</v>
@@ -1694,10 +1939,16 @@
       <c r="D33">
         <v>3.430103</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33">
+        <v>55</v>
+      </c>
+      <c r="F33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B34">
         <v>14.0306681270536</v>
@@ -1708,10 +1959,16 @@
       <c r="D34">
         <v>1.875665</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34">
+        <v>55</v>
+      </c>
+      <c r="F34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B35">
         <v>16.0087623220153</v>
@@ -1722,10 +1979,16 @@
       <c r="D35">
         <v>1.877331</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35">
+        <v>55</v>
+      </c>
+      <c r="F35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B36">
         <v>1.97809419496166</v>
@@ -1736,10 +1999,16 @@
       <c r="D36">
         <v>5.543716</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36">
+        <v>25</v>
+      </c>
+      <c r="F36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B37">
         <v>4.00219058050383</v>
@@ -1750,10 +2019,16 @@
       <c r="D37">
         <v>4.307565</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37">
+        <v>25</v>
+      </c>
+      <c r="F37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B38">
         <v>6.026286966046</v>
@@ -1764,10 +2039,16 @@
       <c r="D38">
         <v>3.690341</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38">
+        <v>25</v>
+      </c>
+      <c r="F38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B39">
         <v>8.02738225629792</v>
@@ -1778,10 +2059,16 @@
       <c r="D39">
         <v>3.090782</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39">
+        <v>25</v>
+      </c>
+      <c r="F39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B40">
         <v>8.9934282584885</v>
@@ -1792,10 +2079,16 @@
       <c r="D40">
         <v>4.028829</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40">
+        <v>25</v>
+      </c>
+      <c r="F40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B41">
         <v>11.0175246440306</v>
@@ -1805,6 +2098,12 @@
       </c>
       <c r="D41">
         <v>1.855444</v>
+      </c>
+      <c r="E41">
+        <v>25</v>
+      </c>
+      <c r="F41" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>